<commit_message>
doc update from Alex
</commit_message>
<xml_diff>
--- a/documents/Backlog.xlsx
+++ b/documents/Backlog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/Current/CO600 Group Project/Documentation/New/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1553D380-083B-B34B-8366-2164779CD26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D56B15-F0A2-46D0-9C53-6DE1E5E506FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Product Backlog'!$B$2:$M$58</definedName>
     <definedName name="Priority">'Agile Product Backlog'!$P$6:$P$8</definedName>
     <definedName name="Status">'Agile Product Backlog'!$Q$6:$Q$8</definedName>
     <definedName name="YesNo">'Agile Product Backlog'!$O$6:$O$7</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="72">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -229,6 +229,33 @@
   </si>
   <si>
     <t>Develop And Implement SQL Code For Android Application.</t>
+  </si>
+  <si>
+    <t>Implement Voice Commands &amp; Air Quality Functionality.</t>
+  </si>
+  <si>
+    <t>Weather API Implementation.</t>
+  </si>
+  <si>
+    <t>Implement Android Pages That Need To Be Implemented.</t>
+  </si>
+  <si>
+    <t>Implement Settings Page Functionality.</t>
+  </si>
+  <si>
+    <t>Binary File Functionality Algorithm.</t>
+  </si>
+  <si>
+    <t>Implement Arduino HTTP Connection.</t>
+  </si>
+  <si>
+    <t>Implement Motion Sensor On Node MCU &amp; Fan Control.</t>
+  </si>
+  <si>
+    <t>Finalise Poster &amp; Abstract</t>
+  </si>
+  <si>
+    <t>Begin Corpus &amp; Technical Manual</t>
   </si>
 </sst>
 </file>
@@ -786,14 +813,14 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI85"/>
+  <dimension ref="B1:AI97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="4" customWidth="1"/>
@@ -812,7 +839,7 @@
     <col min="19" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:35" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
@@ -850,7 +877,7 @@
       <c r="AH1" s="3"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
@@ -910,7 +937,7 @@
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
     </row>
-    <row r="3" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -947,7 +974,7 @@
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
     </row>
-    <row r="4" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7">
         <v>1</v>
       </c>
@@ -1009,7 +1036,7 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
     </row>
-    <row r="5" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>2</v>
       </c>
@@ -1069,7 +1096,7 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>3</v>
       </c>
@@ -1134,7 +1161,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>4</v>
       </c>
@@ -1199,7 +1226,7 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>5</v>
       </c>
@@ -1262,7 +1289,7 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="2:35" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:35" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>6</v>
       </c>
@@ -1321,7 +1348,7 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="10" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>7</v>
       </c>
@@ -1380,7 +1407,7 @@
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>8</v>
       </c>
@@ -1437,7 +1464,7 @@
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>9</v>
       </c>
@@ -1494,7 +1521,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>10</v>
       </c>
@@ -1551,7 +1578,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
@@ -1586,7 +1613,7 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
         <v>1</v>
       </c>
@@ -1643,7 +1670,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
         <v>2</v>
       </c>
@@ -1700,7 +1727,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>3</v>
       </c>
@@ -1757,7 +1784,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
         <v>4</v>
       </c>
@@ -1814,7 +1841,7 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7">
         <v>5</v>
       </c>
@@ -1871,7 +1898,7 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>6</v>
       </c>
@@ -1928,7 +1955,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>7</v>
       </c>
@@ -1985,7 +2012,7 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>8</v>
       </c>
@@ -2042,7 +2069,7 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
         <v>9</v>
       </c>
@@ -2102,7 +2129,7 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>10</v>
       </c>
@@ -2162,7 +2189,7 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
@@ -2200,7 +2227,7 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
         <v>1</v>
       </c>
@@ -2229,7 +2256,7 @@
         <v>7</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L26" s="7">
         <v>50</v>
@@ -2260,7 +2287,7 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7">
         <v>2</v>
       </c>
@@ -2289,7 +2316,7 @@
         <v>7</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L27" s="7">
         <v>50</v>
@@ -2320,7 +2347,7 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="7">
         <v>3</v>
       </c>
@@ -2349,7 +2376,7 @@
         <v>7</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L28" s="7">
         <v>10</v>
@@ -2380,7 +2407,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7">
         <v>4</v>
       </c>
@@ -2409,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L29" s="7">
         <v>10</v>
@@ -2440,7 +2467,7 @@
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="7">
         <v>5</v>
       </c>
@@ -2469,7 +2496,7 @@
         <v>7</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L30" s="7">
         <v>10</v>
@@ -2500,7 +2527,7 @@
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
     </row>
-    <row r="31" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="7">
         <v>6</v>
       </c>
@@ -2529,7 +2556,7 @@
         <v>7</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L31" s="7">
         <v>50</v>
@@ -2560,7 +2587,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
         <v>7</v>
       </c>
@@ -2589,7 +2616,7 @@
         <v>7</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L32" s="7">
         <v>50</v>
@@ -2620,7 +2647,7 @@
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
     </row>
-    <row r="33" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="7">
         <v>8</v>
       </c>
@@ -2649,7 +2676,7 @@
         <v>7</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L33" s="7">
         <v>50</v>
@@ -2680,7 +2707,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="7">
         <v>9</v>
       </c>
@@ -2709,7 +2736,7 @@
         <v>7</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L34" s="7">
         <v>2</v>
@@ -2740,7 +2767,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
@@ -2778,21 +2805,43 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+    <row r="36" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D36" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+      <c r="E36" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G36" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="7">
+        <v>20</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -2816,21 +2865,43 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+    <row r="37" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G37" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="7">
+        <v>50</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -2854,21 +2925,43 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+    <row r="38" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="7">
+        <v>3</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G38" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="7">
+        <v>5</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -2892,21 +2985,43 @@
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
     </row>
-    <row r="39" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5" t="s">
+    <row r="39" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="7">
         <v>4</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
+      <c r="C39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G39" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="7">
+        <v>20</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -2930,21 +3045,43 @@
       <c r="AH39" s="3"/>
       <c r="AI39" s="3"/>
     </row>
-    <row r="40" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+    <row r="40" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="7">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G40" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="7">
+        <v>10</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -2968,21 +3105,43 @@
       <c r="AH40" s="3"/>
       <c r="AI40" s="3"/>
     </row>
-    <row r="41" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+    <row r="41" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="7">
+        <v>6</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G41" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="7">
+        <v>30</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -3006,21 +3165,43 @@
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
     </row>
-    <row r="42" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+    <row r="42" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="7">
+        <v>7</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G42" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" s="7">
+        <v>50</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -3044,21 +3225,43 @@
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
     </row>
-    <row r="43" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
+    <row r="43" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="7">
+        <v>8</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G43" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" s="7">
+        <v>15</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -3082,21 +3285,43 @@
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
     </row>
-    <row r="44" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+    <row r="44" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="7">
+        <v>9</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="8">
+        <v>44211</v>
+      </c>
+      <c r="G44" s="8">
+        <v>44242</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" s="7">
+        <v>50</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -3120,21 +3345,21 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
     </row>
-    <row r="45" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
+    <row r="45" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -3158,8 +3383,10 @@
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
     </row>
-    <row r="46" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="7"/>
+    <row r="46" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="7">
+        <v>1</v>
+      </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7" t="s">
         <v>26</v>
@@ -3170,9 +3397,13 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
+      <c r="K46" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
+      <c r="M46" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -3196,18 +3427,27 @@
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
     </row>
-    <row r="47" spans="2:35" ht="10" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
+    <row r="47" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="7">
+        <v>2</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -3231,54 +3471,71 @@
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
     </row>
-    <row r="48" spans="2:35" s="12" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="11"/>
-      <c r="W48" s="11"/>
-      <c r="X48" s="11"/>
-      <c r="Y48" s="11"/>
-      <c r="Z48" s="11"/>
-      <c r="AA48" s="11"/>
-      <c r="AB48" s="11"/>
-      <c r="AC48" s="11"/>
-      <c r="AD48" s="11"/>
-      <c r="AE48" s="11"/>
-      <c r="AF48" s="11"/>
-      <c r="AG48" s="11"/>
-      <c r="AH48" s="11"/>
-      <c r="AI48" s="11"/>
-    </row>
-    <row r="49" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
+    <row r="48" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="7">
+        <v>3</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+    </row>
+    <row r="49" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="7">
+        <v>4</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
@@ -3302,18 +3559,27 @@
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
     </row>
-    <row r="50" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+    <row r="50" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="7">
+        <v>5</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
@@ -3337,18 +3603,27 @@
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
     </row>
-    <row r="51" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
+    <row r="51" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="7">
+        <v>6</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
@@ -3372,18 +3647,27 @@
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
     </row>
-    <row r="52" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
+    <row r="52" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="7">
+        <v>7</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
@@ -3407,18 +3691,27 @@
       <c r="AH52" s="3"/>
       <c r="AI52" s="3"/>
     </row>
-    <row r="53" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
+    <row r="53" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="7">
+        <v>8</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
@@ -3442,18 +3735,27 @@
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
     </row>
-    <row r="54" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
+    <row r="54" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="7">
+        <v>9</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
@@ -3477,18 +3779,21 @@
       <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
     </row>
-    <row r="55" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+    <row r="55" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
@@ -3512,18 +3817,21 @@
       <c r="AH55" s="3"/>
       <c r="AI55" s="3"/>
     </row>
-    <row r="56" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
+    <row r="56" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
@@ -3547,18 +3855,21 @@
       <c r="AH56" s="3"/>
       <c r="AI56" s="3"/>
     </row>
-    <row r="57" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
+    <row r="57" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
@@ -3582,18 +3893,21 @@
       <c r="AH57" s="3"/>
       <c r="AI57" s="3"/>
     </row>
-    <row r="58" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
+    <row r="58" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
@@ -3617,7 +3931,7 @@
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
     </row>
-    <row r="59" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:35" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -3652,42 +3966,43 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
     </row>
-    <row r="60" spans="3:35" x14ac:dyDescent="0.2">
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
-      <c r="X60" s="3"/>
-      <c r="Y60" s="3"/>
-      <c r="Z60" s="3"/>
-      <c r="AA60" s="3"/>
-      <c r="AB60" s="3"/>
-      <c r="AC60" s="3"/>
-      <c r="AD60" s="3"/>
-      <c r="AE60" s="3"/>
-      <c r="AF60" s="3"/>
-      <c r="AG60" s="3"/>
-      <c r="AH60" s="3"/>
-      <c r="AI60" s="3"/>
-    </row>
-    <row r="61" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:35" s="12" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B60" s="15"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+      <c r="W60" s="11"/>
+      <c r="X60" s="11"/>
+      <c r="Y60" s="11"/>
+      <c r="Z60" s="11"/>
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="11"/>
+      <c r="AC60" s="11"/>
+      <c r="AD60" s="11"/>
+      <c r="AE60" s="11"/>
+      <c r="AF60" s="11"/>
+      <c r="AG60" s="11"/>
+      <c r="AH60" s="11"/>
+      <c r="AI60" s="11"/>
+    </row>
+    <row r="61" spans="2:35" x14ac:dyDescent="0.35">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -3722,7 +4037,7 @@
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
     </row>
-    <row r="62" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:35" x14ac:dyDescent="0.35">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3757,7 +4072,7 @@
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
     </row>
-    <row r="63" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:35" x14ac:dyDescent="0.35">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -3792,7 +4107,7 @@
       <c r="AH63" s="3"/>
       <c r="AI63" s="3"/>
     </row>
-    <row r="64" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:35" x14ac:dyDescent="0.35">
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3827,7 +4142,7 @@
       <c r="AH64" s="3"/>
       <c r="AI64" s="3"/>
     </row>
-    <row r="65" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -3862,7 +4177,7 @@
       <c r="AH65" s="3"/>
       <c r="AI65" s="3"/>
     </row>
-    <row r="66" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3897,7 +4212,7 @@
       <c r="AH66" s="3"/>
       <c r="AI66" s="3"/>
     </row>
-    <row r="67" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -3932,7 +4247,7 @@
       <c r="AH67" s="3"/>
       <c r="AI67" s="3"/>
     </row>
-    <row r="68" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -3967,7 +4282,7 @@
       <c r="AH68" s="3"/>
       <c r="AI68" s="3"/>
     </row>
-    <row r="69" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -4002,7 +4317,7 @@
       <c r="AH69" s="3"/>
       <c r="AI69" s="3"/>
     </row>
-    <row r="70" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -4037,7 +4352,7 @@
       <c r="AH70" s="3"/>
       <c r="AI70" s="3"/>
     </row>
-    <row r="71" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -4072,7 +4387,7 @@
       <c r="AH71" s="3"/>
       <c r="AI71" s="3"/>
     </row>
-    <row r="72" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -4107,7 +4422,7 @@
       <c r="AH72" s="3"/>
       <c r="AI72" s="3"/>
     </row>
-    <row r="73" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -4142,7 +4457,7 @@
       <c r="AH73" s="3"/>
       <c r="AI73" s="3"/>
     </row>
-    <row r="74" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -4177,7 +4492,7 @@
       <c r="AH74" s="3"/>
       <c r="AI74" s="3"/>
     </row>
-    <row r="75" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
@@ -4212,7 +4527,7 @@
       <c r="AH75" s="3"/>
       <c r="AI75" s="3"/>
     </row>
-    <row r="76" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -4247,7 +4562,7 @@
       <c r="AH76" s="3"/>
       <c r="AI76" s="3"/>
     </row>
-    <row r="77" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -4282,7 +4597,7 @@
       <c r="AH77" s="3"/>
       <c r="AI77" s="3"/>
     </row>
-    <row r="78" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -4317,7 +4632,7 @@
       <c r="AH78" s="3"/>
       <c r="AI78" s="3"/>
     </row>
-    <row r="79" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -4352,7 +4667,7 @@
       <c r="AH79" s="3"/>
       <c r="AI79" s="3"/>
     </row>
-    <row r="80" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -4387,7 +4702,7 @@
       <c r="AH80" s="3"/>
       <c r="AI80" s="3"/>
     </row>
-    <row r="81" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -4422,7 +4737,7 @@
       <c r="AH81" s="3"/>
       <c r="AI81" s="3"/>
     </row>
-    <row r="82" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -4457,7 +4772,7 @@
       <c r="AH82" s="3"/>
       <c r="AI82" s="3"/>
     </row>
-    <row r="83" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -4492,7 +4807,7 @@
       <c r="AH83" s="3"/>
       <c r="AI83" s="3"/>
     </row>
-    <row r="84" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -4527,7 +4842,7 @@
       <c r="AH84" s="3"/>
       <c r="AI84" s="3"/>
     </row>
-    <row r="85" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:35" x14ac:dyDescent="0.35">
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -4562,26 +4877,446 @@
       <c r="AH85" s="3"/>
       <c r="AI85" s="3"/>
     </row>
+    <row r="86" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
+      <c r="X86" s="3"/>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3"/>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3"/>
+      <c r="AC86" s="3"/>
+      <c r="AD86" s="3"/>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+    </row>
+    <row r="87" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
+      <c r="V87" s="3"/>
+      <c r="W87" s="3"/>
+      <c r="X87" s="3"/>
+      <c r="Y87" s="3"/>
+      <c r="Z87" s="3"/>
+      <c r="AA87" s="3"/>
+      <c r="AB87" s="3"/>
+      <c r="AC87" s="3"/>
+      <c r="AD87" s="3"/>
+      <c r="AE87" s="3"/>
+      <c r="AF87" s="3"/>
+      <c r="AG87" s="3"/>
+      <c r="AH87" s="3"/>
+      <c r="AI87" s="3"/>
+    </row>
+    <row r="88" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="3"/>
+      <c r="W88" s="3"/>
+      <c r="X88" s="3"/>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3"/>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3"/>
+      <c r="AC88" s="3"/>
+      <c r="AD88" s="3"/>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+    </row>
+    <row r="89" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="U89" s="3"/>
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+      <c r="X89" s="3"/>
+      <c r="Y89" s="3"/>
+      <c r="Z89" s="3"/>
+      <c r="AA89" s="3"/>
+      <c r="AB89" s="3"/>
+      <c r="AC89" s="3"/>
+      <c r="AD89" s="3"/>
+      <c r="AE89" s="3"/>
+      <c r="AF89" s="3"/>
+      <c r="AG89" s="3"/>
+      <c r="AH89" s="3"/>
+      <c r="AI89" s="3"/>
+    </row>
+    <row r="90" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+      <c r="X90" s="3"/>
+      <c r="Y90" s="3"/>
+      <c r="Z90" s="3"/>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3"/>
+      <c r="AC90" s="3"/>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+    </row>
+    <row r="91" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+      <c r="X91" s="3"/>
+      <c r="Y91" s="3"/>
+      <c r="Z91" s="3"/>
+      <c r="AA91" s="3"/>
+      <c r="AB91" s="3"/>
+      <c r="AC91" s="3"/>
+      <c r="AD91" s="3"/>
+      <c r="AE91" s="3"/>
+      <c r="AF91" s="3"/>
+      <c r="AG91" s="3"/>
+      <c r="AH91" s="3"/>
+      <c r="AI91" s="3"/>
+    </row>
+    <row r="92" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+      <c r="X92" s="3"/>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3"/>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3"/>
+      <c r="AC92" s="3"/>
+      <c r="AD92" s="3"/>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+    </row>
+    <row r="93" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="3"/>
+      <c r="T93" s="3"/>
+      <c r="U93" s="3"/>
+      <c r="V93" s="3"/>
+      <c r="W93" s="3"/>
+      <c r="X93" s="3"/>
+      <c r="Y93" s="3"/>
+      <c r="Z93" s="3"/>
+      <c r="AA93" s="3"/>
+      <c r="AB93" s="3"/>
+      <c r="AC93" s="3"/>
+      <c r="AD93" s="3"/>
+      <c r="AE93" s="3"/>
+      <c r="AF93" s="3"/>
+      <c r="AG93" s="3"/>
+      <c r="AH93" s="3"/>
+      <c r="AI93" s="3"/>
+    </row>
+    <row r="94" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="3"/>
+      <c r="T94" s="3"/>
+      <c r="U94" s="3"/>
+      <c r="V94" s="3"/>
+      <c r="W94" s="3"/>
+      <c r="X94" s="3"/>
+      <c r="Y94" s="3"/>
+      <c r="Z94" s="3"/>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3"/>
+      <c r="AC94" s="3"/>
+      <c r="AD94" s="3"/>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+    </row>
+    <row r="95" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="3"/>
+      <c r="T95" s="3"/>
+      <c r="U95" s="3"/>
+      <c r="V95" s="3"/>
+      <c r="W95" s="3"/>
+      <c r="X95" s="3"/>
+      <c r="Y95" s="3"/>
+      <c r="Z95" s="3"/>
+      <c r="AA95" s="3"/>
+      <c r="AB95" s="3"/>
+      <c r="AC95" s="3"/>
+      <c r="AD95" s="3"/>
+      <c r="AE95" s="3"/>
+      <c r="AF95" s="3"/>
+      <c r="AG95" s="3"/>
+      <c r="AH95" s="3"/>
+      <c r="AI95" s="3"/>
+    </row>
+    <row r="96" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="3"/>
+      <c r="V96" s="3"/>
+      <c r="W96" s="3"/>
+      <c r="X96" s="3"/>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3"/>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3"/>
+      <c r="AC96" s="3"/>
+      <c r="AD96" s="3"/>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+    </row>
+    <row r="97" spans="3:35" x14ac:dyDescent="0.35">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
+      <c r="P97" s="3"/>
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="U97" s="3"/>
+      <c r="V97" s="3"/>
+      <c r="W97" s="3"/>
+      <c r="X97" s="3"/>
+      <c r="Y97" s="3"/>
+      <c r="Z97" s="3"/>
+      <c r="AA97" s="3"/>
+      <c r="AB97" s="3"/>
+      <c r="AC97" s="3"/>
+      <c r="AD97" s="3"/>
+      <c r="AE97" s="3"/>
+      <c r="AF97" s="3"/>
+      <c r="AG97" s="3"/>
+      <c r="AH97" s="3"/>
+      <c r="AI97" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B48:M48"/>
+    <mergeCell ref="B60:M60"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I46 M3:M46" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M58 H3:I58" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J46" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J58" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K46" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K58" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$A$13:$A$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44:E46 E26:E34 E15:E24 E4:E13 E36:E38 E40:E42" xr:uid="{84E655FD-F32C-8A43-9CD3-B2D10FECBBDB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E56:E58 E26:E34 E15:E24 E4:E13 E36:E44 E46:E54" xr:uid="{84E655FD-F32C-8A43-9CD3-B2D10FECBBDB}">
       <formula1>$R$6:$R$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>